<commit_message>
business report finished (i think, i hope)
</commit_message>
<xml_diff>
--- a/0000_Docs/0000_Report/LoRaSnow_report/Docs/PlanningPrevu.xlsx
+++ b/0000_Docs/0000_Report/LoRaSnow_report/Docs/PlanningPrevu.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e675ddd269f32ab/Documents/3e/PGA/git/LoRaSnow/0000_Docs/0000_Report/LoRaSnow_report/Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\LoRaSnow\0000_Docs\0000_Report\LoRaSnow_report\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{D6E8EA68-F48B-474B-8AD8-B45E9514ABA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A8850D7-85CD-44EC-A26A-E74D3A2E4CA6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624B5C81-A654-4557-8FFB-88FECCF924E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{C469FEE3-4799-45B8-9D7F-3F6FA63AB014}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C469FEE3-4799-45B8-9D7F-3F6FA63AB014}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -762,20 +762,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5DBF098-45F6-4E51-869D-FA0694BD3957}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" style="2" customWidth="1"/>
-    <col min="2" max="19" width="4" style="3" customWidth="1"/>
-    <col min="20" max="16384" width="10.6640625" style="3"/>
+    <col min="1" max="1" width="26.7109375" style="2" customWidth="1"/>
+    <col min="2" max="19" width="8.5703125" style="3" customWidth="1"/>
+    <col min="20" max="16384" width="10.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>5</v>
       </c>
@@ -834,7 +837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -857,7 +860,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="17"/>
     </row>
-    <row r="3" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>6</v>
       </c>
@@ -880,7 +883,7 @@
       <c r="R3" s="5"/>
       <c r="S3" s="17"/>
     </row>
-    <row r="4" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -903,7 +906,7 @@
       <c r="R4" s="9"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>7</v>
       </c>
@@ -926,7 +929,7 @@
       <c r="R5" s="5"/>
       <c r="S5" s="17"/>
     </row>
-    <row r="6" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>8</v>
       </c>
@@ -949,7 +952,7 @@
       <c r="R6" s="5"/>
       <c r="S6" s="17"/>
     </row>
-    <row r="7" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>9</v>
       </c>
@@ -972,7 +975,7 @@
       <c r="R7" s="27"/>
       <c r="S7" s="17"/>
     </row>
-    <row r="8" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>16</v>
       </c>
@@ -995,7 +998,7 @@
       <c r="R8" s="27"/>
       <c r="S8" s="17"/>
     </row>
-    <row r="9" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
@@ -1018,7 +1021,7 @@
       <c r="R9" s="11"/>
       <c r="S9" s="12"/>
     </row>
-    <row r="10" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>10</v>
       </c>
@@ -1041,7 +1044,7 @@
       <c r="R10" s="24"/>
       <c r="S10" s="17"/>
     </row>
-    <row r="11" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -1064,7 +1067,7 @@
       <c r="R11" s="6"/>
       <c r="S11" s="7"/>
     </row>
-    <row r="12" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>11</v>
       </c>
@@ -1087,7 +1090,7 @@
       <c r="R12" s="24"/>
       <c r="S12" s="17"/>
     </row>
-    <row r="13" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>12</v>
       </c>
@@ -1110,7 +1113,7 @@
       <c r="R13" s="24"/>
       <c r="S13" s="17"/>
     </row>
-    <row r="14" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>2</v>
       </c>
@@ -1133,7 +1136,7 @@
       <c r="R14" s="32"/>
       <c r="S14" s="33"/>
     </row>
-    <row r="15" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>13</v>
       </c>
@@ -1156,7 +1159,7 @@
       <c r="R15" s="30"/>
       <c r="S15" s="31"/>
     </row>
-    <row r="16" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>14</v>
       </c>
@@ -1179,7 +1182,7 @@
       <c r="R16" s="30"/>
       <c r="S16" s="31"/>
     </row>
-    <row r="17" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:19" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>15</v>
       </c>
@@ -1203,7 +1206,7 @@
       <c r="S17" s="31"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="78" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>